<commit_message>
Added actual whitepaper, and edited data spreadsheet
</commit_message>
<xml_diff>
--- a/whitepaperExperimenting.xlsx
+++ b/whitepaperExperimenting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5fa63845bd084c5/Documents/BYUI Stuff/Winter 2021/CS345/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_946C2C748E109164B2B6FDF6C48870E449CDCA55" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F810AB52-2436-4AFD-BB33-9EB21DFFA396}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_946C2C748E109164B2B6FDF6C48870E449CDCA55" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{39CC506F-6077-4CFA-8BC8-3EC660A92EE3}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4140" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="24">
   <si>
     <t>LinuxLab (2 cores, 4 thread)</t>
   </si>
@@ -90,6 +90,9 @@
   <si>
     <t>LinuxLab, extended io research</t>
   </si>
+  <si>
+    <t>Michael's computer, extended io research</t>
+  </si>
 </sst>
 </file>
 
@@ -148,13 +151,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1720,7 +1724,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Michael's CPU intensive results</a:t>
+              <a:t>Michael's CPU-intensive results</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6422,6 +6426,232 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B4DF-4E16-873C-ECDECF3AB875}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Michael's</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$166:$D$229</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>53.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.270000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.4600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.47</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.0500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.31</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.2100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.89</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.08</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.41</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.7699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.58</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.18</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.27</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.1900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.17</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.51</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.03</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.1900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.86</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.61</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.79</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.51</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.6100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.51</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.57</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DC67-44A3-86D9-77F652E67B00}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11091,8 +11321,8 @@
   </sheetPr>
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11127,21 +11357,21 @@
       <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="7" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="9" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -11973,21 +12203,21 @@
       <c r="H22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="7" t="s">
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="9" t="s">
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -12822,21 +13052,21 @@
       <c r="H42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I42" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="7" t="s">
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="9" t="s">
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -13668,21 +13898,21 @@
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="G62" s="2"/>
-      <c r="I62" s="7" t="s">
+      <c r="I62" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="7" t="s">
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M62" s="8"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="9" t="s">
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+      <c r="O62" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
+      <c r="P62" s="9"/>
+      <c r="Q62" s="9"/>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -14517,21 +14747,21 @@
       </c>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="I82" s="7" t="s">
+      <c r="I82" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J82" s="8"/>
-      <c r="K82" s="8"/>
-      <c r="L82" s="7" t="s">
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M82" s="8"/>
-      <c r="N82" s="8"/>
-      <c r="O82" s="9" t="s">
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+      <c r="O82" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P82" s="8"/>
-      <c r="Q82" s="8"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="9"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
@@ -16285,7 +16515,7 @@
       </c>
       <c r="G160" s="2"/>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B161" s="2"/>
       <c r="C161" s="6">
         <v>61</v>
@@ -16301,7 +16531,7 @@
       </c>
       <c r="G161" s="2"/>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B162" s="2"/>
       <c r="C162" s="6">
         <v>62</v>
@@ -16317,7 +16547,7 @@
       </c>
       <c r="G162" s="2"/>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B163" s="2"/>
       <c r="C163" s="6">
         <v>63</v>
@@ -16333,7 +16563,7 @@
       </c>
       <c r="G163" s="2"/>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B164" s="2"/>
       <c r="C164" s="6">
         <v>64</v>
@@ -16349,264 +16579,1035 @@
       </c>
       <c r="G164" s="2"/>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B165" s="2"/>
       <c r="G165" s="2"/>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="B166" s="2"/>
+      <c r="C166" s="7">
+        <v>1</v>
+      </c>
+      <c r="D166" s="7">
+        <v>53.32</v>
+      </c>
+      <c r="E166" s="7">
+        <v>0</v>
+      </c>
+      <c r="F166" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G166" s="2"/>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B167" s="2"/>
+      <c r="C167" s="7">
+        <v>2</v>
+      </c>
+      <c r="D167" s="7">
+        <v>36.270000000000003</v>
+      </c>
+      <c r="E167" s="7">
+        <v>0</v>
+      </c>
+      <c r="F167" s="7">
+        <v>0</v>
+      </c>
       <c r="G167" s="2"/>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B168" s="2"/>
+      <c r="C168" s="7">
+        <v>3</v>
+      </c>
+      <c r="D168" s="7">
+        <v>22.68</v>
+      </c>
+      <c r="E168" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F168" s="7">
+        <v>0</v>
+      </c>
       <c r="G168" s="2"/>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B169" s="2"/>
+      <c r="C169" s="7">
+        <v>4</v>
+      </c>
+      <c r="D169" s="7">
+        <v>19.27</v>
+      </c>
+      <c r="E169" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F169" s="7">
+        <v>0</v>
+      </c>
       <c r="G169" s="2"/>
     </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B170" s="2"/>
+      <c r="C170" s="7">
+        <v>5</v>
+      </c>
+      <c r="D170" s="7">
+        <v>13.46</v>
+      </c>
+      <c r="E170" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F170" s="7">
+        <v>0</v>
+      </c>
       <c r="G170" s="2"/>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B171" s="2"/>
+      <c r="C171" s="7">
+        <v>6</v>
+      </c>
+      <c r="D171" s="7">
+        <v>13.8</v>
+      </c>
+      <c r="E171" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F171" s="7">
+        <v>0</v>
+      </c>
       <c r="G171" s="2"/>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B172" s="2"/>
+      <c r="C172" s="7">
+        <v>7</v>
+      </c>
+      <c r="D172" s="7">
+        <v>13.14</v>
+      </c>
+      <c r="E172" s="7">
+        <v>0</v>
+      </c>
+      <c r="F172" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G172" s="2"/>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B173" s="2"/>
+      <c r="C173" s="7">
+        <v>8</v>
+      </c>
+      <c r="D173" s="7">
+        <v>12.3</v>
+      </c>
+      <c r="E173" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F173" s="7">
+        <v>0</v>
+      </c>
       <c r="G173" s="2"/>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B174" s="2"/>
+      <c r="C174" s="7">
+        <v>9</v>
+      </c>
+      <c r="D174" s="7">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="E174" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F174" s="7">
+        <v>0</v>
+      </c>
       <c r="G174" s="2"/>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B175" s="2"/>
+      <c r="C175" s="7">
+        <v>10</v>
+      </c>
+      <c r="D175" s="7">
+        <v>9.09</v>
+      </c>
+      <c r="E175" s="7">
+        <v>0</v>
+      </c>
+      <c r="F175" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G175" s="2"/>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B176" s="2"/>
+      <c r="C176" s="7">
+        <v>11</v>
+      </c>
+      <c r="D176" s="7">
+        <v>7.47</v>
+      </c>
+      <c r="E176" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F176" s="7">
+        <v>0</v>
+      </c>
       <c r="G176" s="2"/>
     </row>
     <row r="177" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B177" s="2"/>
+      <c r="C177" s="7">
+        <v>12</v>
+      </c>
+      <c r="D177" s="7">
+        <v>7.32</v>
+      </c>
+      <c r="E177" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F177" s="7">
+        <v>0</v>
+      </c>
       <c r="G177" s="2"/>
     </row>
     <row r="178" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B178" s="2"/>
+      <c r="C178" s="7">
+        <v>13</v>
+      </c>
+      <c r="D178" s="7">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="E178" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="F178" s="7">
+        <v>0.32</v>
+      </c>
       <c r="G178" s="2"/>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B179" s="2"/>
+      <c r="C179" s="7">
+        <v>14</v>
+      </c>
+      <c r="D179" s="7">
+        <v>7.31</v>
+      </c>
+      <c r="E179" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F179" s="7">
+        <v>0</v>
+      </c>
       <c r="G179" s="2"/>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B180" s="2"/>
+      <c r="C180" s="7">
+        <v>15</v>
+      </c>
+      <c r="D180" s="7">
+        <v>7.16</v>
+      </c>
+      <c r="E180" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F180" s="7">
+        <v>0</v>
+      </c>
       <c r="G180" s="2"/>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181" s="2"/>
+      <c r="C181" s="7">
+        <v>16</v>
+      </c>
+      <c r="D181" s="7">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="E181" s="7">
+        <v>0</v>
+      </c>
+      <c r="F181" s="7">
+        <v>0</v>
+      </c>
       <c r="G181" s="2"/>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B182" s="2"/>
+      <c r="C182" s="7">
+        <v>17</v>
+      </c>
+      <c r="D182" s="7">
+        <v>6.25</v>
+      </c>
+      <c r="E182" s="7">
+        <v>0</v>
+      </c>
+      <c r="F182" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G182" s="2"/>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B183" s="2"/>
+      <c r="C183" s="7">
+        <v>18</v>
+      </c>
+      <c r="D183" s="7">
+        <v>5.32</v>
+      </c>
+      <c r="E183" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F183" s="7">
+        <v>0</v>
+      </c>
       <c r="G183" s="2"/>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B184" s="2"/>
+      <c r="C184" s="7">
+        <v>19</v>
+      </c>
+      <c r="D184" s="7">
+        <v>5.89</v>
+      </c>
+      <c r="E184" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F184" s="7">
+        <v>0</v>
+      </c>
       <c r="G184" s="2"/>
     </row>
     <row r="185" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B185" s="2"/>
+      <c r="C185" s="7">
+        <v>20</v>
+      </c>
+      <c r="D185" s="7">
+        <v>5.29</v>
+      </c>
+      <c r="E185" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F185" s="7">
+        <v>0</v>
+      </c>
       <c r="G185" s="2"/>
     </row>
     <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B186" s="2"/>
+      <c r="C186" s="7">
+        <v>21</v>
+      </c>
+      <c r="D186" s="7">
+        <v>6.25</v>
+      </c>
+      <c r="E186" s="7">
+        <v>0</v>
+      </c>
+      <c r="F186" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G186" s="2"/>
     </row>
     <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B187" s="2"/>
+      <c r="C187" s="7">
+        <v>22</v>
+      </c>
+      <c r="D187" s="7">
+        <v>6.08</v>
+      </c>
+      <c r="E187" s="7">
+        <v>0</v>
+      </c>
+      <c r="F187" s="7">
+        <v>0</v>
+      </c>
       <c r="G187" s="2"/>
     </row>
     <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B188" s="2"/>
+      <c r="C188" s="7">
+        <v>23</v>
+      </c>
+      <c r="D188" s="7">
+        <v>5.41</v>
+      </c>
+      <c r="E188" s="7">
+        <v>0</v>
+      </c>
+      <c r="F188" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G188" s="2"/>
     </row>
     <row r="189" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B189" s="2"/>
+      <c r="C189" s="7">
+        <v>24</v>
+      </c>
+      <c r="D189" s="7">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="E189" s="7">
+        <v>0</v>
+      </c>
+      <c r="F189" s="7">
+        <v>0</v>
+      </c>
       <c r="G189" s="2"/>
     </row>
     <row r="190" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B190" s="2"/>
+      <c r="C190" s="7">
+        <v>25</v>
+      </c>
+      <c r="D190" s="7">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="E190" s="7">
+        <v>0</v>
+      </c>
+      <c r="F190" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G190" s="2"/>
     </row>
     <row r="191" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B191" s="2"/>
+      <c r="C191" s="7">
+        <v>26</v>
+      </c>
+      <c r="D191" s="7">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E191" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F191" s="7">
+        <v>0</v>
+      </c>
       <c r="G191" s="2"/>
     </row>
     <row r="192" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B192" s="2"/>
+      <c r="C192" s="7">
+        <v>27</v>
+      </c>
+      <c r="D192" s="7">
+        <v>3.58</v>
+      </c>
+      <c r="E192" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F192" s="7">
+        <v>0</v>
+      </c>
       <c r="G192" s="2"/>
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193" s="2"/>
+      <c r="C193" s="7">
+        <v>28</v>
+      </c>
+      <c r="D193" s="7">
+        <v>4.63</v>
+      </c>
+      <c r="E193" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F193" s="7">
+        <v>0</v>
+      </c>
       <c r="G193" s="2"/>
     </row>
     <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="2"/>
+      <c r="C194" s="7">
+        <v>29</v>
+      </c>
+      <c r="D194" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="E194" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F194" s="7">
+        <v>0</v>
+      </c>
       <c r="G194" s="2"/>
     </row>
     <row r="195" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B195" s="2"/>
+      <c r="C195" s="7">
+        <v>30</v>
+      </c>
+      <c r="D195" s="7">
+        <v>4.18</v>
+      </c>
+      <c r="E195" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F195" s="7">
+        <v>0</v>
+      </c>
       <c r="G195" s="2"/>
     </row>
     <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196" s="2"/>
+      <c r="C196" s="7">
+        <v>31</v>
+      </c>
+      <c r="D196" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="E196" s="7">
+        <v>0</v>
+      </c>
+      <c r="F196" s="7">
+        <v>0.02</v>
+      </c>
       <c r="G196" s="2"/>
     </row>
     <row r="197" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B197" s="2"/>
+      <c r="C197" s="7">
+        <v>32</v>
+      </c>
+      <c r="D197" s="7">
+        <v>5.27</v>
+      </c>
+      <c r="E197" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F197" s="7">
+        <v>0</v>
+      </c>
       <c r="G197" s="2"/>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B198" s="2"/>
+      <c r="C198" s="7">
+        <v>33</v>
+      </c>
+      <c r="D198" s="7">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E198" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F198" s="7">
+        <v>0</v>
+      </c>
       <c r="G198" s="2"/>
     </row>
     <row r="199" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B199" s="2"/>
+      <c r="C199" s="7">
+        <v>34</v>
+      </c>
+      <c r="D199" s="7">
+        <v>4.17</v>
+      </c>
+      <c r="E199" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F199" s="7">
+        <v>0</v>
+      </c>
       <c r="G199" s="2"/>
     </row>
     <row r="200" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B200" s="2"/>
+      <c r="C200" s="7">
+        <v>35</v>
+      </c>
+      <c r="D200" s="7">
+        <v>4.51</v>
+      </c>
+      <c r="E200" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F200" s="7">
+        <v>0</v>
+      </c>
       <c r="G200" s="2"/>
     </row>
     <row r="201" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B201" s="2"/>
+      <c r="C201" s="7">
+        <v>36</v>
+      </c>
+      <c r="D201" s="7">
+        <v>4.63</v>
+      </c>
+      <c r="E201" s="7">
+        <v>0</v>
+      </c>
+      <c r="F201" s="7">
+        <v>0.02</v>
+      </c>
       <c r="G201" s="2"/>
     </row>
     <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" s="2"/>
+      <c r="C202" s="7">
+        <v>37</v>
+      </c>
+      <c r="D202" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="E202" s="7">
+        <v>0</v>
+      </c>
+      <c r="F202" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G202" s="2"/>
     </row>
     <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B203" s="2"/>
+      <c r="C203" s="7">
+        <v>38</v>
+      </c>
+      <c r="D203" s="7">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E203" s="7">
+        <v>0</v>
+      </c>
+      <c r="F203" s="7">
+        <v>0</v>
+      </c>
       <c r="G203" s="2"/>
     </row>
     <row r="204" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B204" s="2"/>
+      <c r="C204" s="7">
+        <v>39</v>
+      </c>
+      <c r="D204" s="7">
+        <v>5.37</v>
+      </c>
+      <c r="E204" s="7">
+        <v>0</v>
+      </c>
+      <c r="F204" s="7">
+        <v>0.02</v>
+      </c>
       <c r="G204" s="2"/>
     </row>
     <row r="205" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B205" s="2"/>
+      <c r="C205" s="7">
+        <v>40</v>
+      </c>
+      <c r="D205" s="7">
+        <v>4.03</v>
+      </c>
+      <c r="E205" s="7">
+        <v>0</v>
+      </c>
+      <c r="F205" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G205" s="2"/>
     </row>
     <row r="206" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B206" s="2"/>
+      <c r="C206" s="7">
+        <v>41</v>
+      </c>
+      <c r="D206" s="7">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E206" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F206" s="7">
+        <v>0</v>
+      </c>
       <c r="G206" s="2"/>
     </row>
     <row r="207" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B207" s="2"/>
+      <c r="C207" s="7">
+        <v>42</v>
+      </c>
+      <c r="D207" s="7">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E207" s="7">
+        <v>0</v>
+      </c>
+      <c r="F207" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G207" s="2"/>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B208" s="2"/>
+      <c r="C208" s="7">
+        <v>43</v>
+      </c>
+      <c r="D208" s="7">
+        <v>3.61</v>
+      </c>
+      <c r="E208" s="7">
+        <v>0</v>
+      </c>
+      <c r="F208" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G208" s="2"/>
     </row>
     <row r="209" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B209" s="2"/>
+      <c r="C209" s="7">
+        <v>44</v>
+      </c>
+      <c r="D209" s="7">
+        <v>3.86</v>
+      </c>
+      <c r="E209" s="7">
+        <v>0</v>
+      </c>
+      <c r="F209" s="7">
+        <v>0.02</v>
+      </c>
       <c r="G209" s="2"/>
     </row>
     <row r="210" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B210" s="2"/>
+      <c r="C210" s="7">
+        <v>45</v>
+      </c>
+      <c r="D210" s="7">
+        <v>5.61</v>
+      </c>
+      <c r="E210" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F210" s="7">
+        <v>0</v>
+      </c>
       <c r="G210" s="2"/>
     </row>
     <row r="211" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B211" s="2"/>
+      <c r="C211" s="7">
+        <v>46</v>
+      </c>
+      <c r="D211" s="7">
+        <v>3.79</v>
+      </c>
+      <c r="E211" s="7">
+        <v>0</v>
+      </c>
+      <c r="F211" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G211" s="2"/>
     </row>
     <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B212" s="2"/>
+      <c r="C212" s="7">
+        <v>47</v>
+      </c>
+      <c r="D212" s="7">
+        <v>4.51</v>
+      </c>
+      <c r="E212" s="7">
+        <v>0</v>
+      </c>
+      <c r="F212" s="7">
+        <v>0.02</v>
+      </c>
       <c r="G212" s="2"/>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B213" s="2"/>
+      <c r="C213" s="7">
+        <v>48</v>
+      </c>
+      <c r="D213" s="7">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E213" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F213" s="7">
+        <v>0</v>
+      </c>
       <c r="G213" s="2"/>
     </row>
     <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B214" s="2"/>
+      <c r="C214" s="7">
+        <v>49</v>
+      </c>
+      <c r="D214" s="7">
+        <v>4.97</v>
+      </c>
+      <c r="E214" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F214" s="7">
+        <v>0</v>
+      </c>
       <c r="G214" s="2"/>
     </row>
     <row r="215" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B215" s="2"/>
+      <c r="C215" s="7">
+        <v>50</v>
+      </c>
+      <c r="D215" s="7">
+        <v>3.51</v>
+      </c>
+      <c r="E215" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F215" s="7">
+        <v>0</v>
+      </c>
       <c r="G215" s="2"/>
     </row>
     <row r="216" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B216" s="2"/>
+      <c r="C216" s="7">
+        <v>51</v>
+      </c>
+      <c r="D216" s="7">
+        <v>4.25</v>
+      </c>
+      <c r="E216" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F216" s="7">
+        <v>0</v>
+      </c>
       <c r="G216" s="2"/>
     </row>
     <row r="217" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B217" s="2"/>
+      <c r="C217" s="7">
+        <v>52</v>
+      </c>
+      <c r="D217" s="7">
+        <v>3.75</v>
+      </c>
+      <c r="E217" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F217" s="7">
+        <v>0</v>
+      </c>
       <c r="G217" s="2"/>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B218" s="2"/>
+      <c r="C218" s="7">
+        <v>53</v>
+      </c>
+      <c r="D218" s="7">
+        <v>4.38</v>
+      </c>
+      <c r="E218" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F218" s="7">
+        <v>0</v>
+      </c>
       <c r="G218" s="2"/>
     </row>
     <row r="219" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B219" s="2"/>
+      <c r="C219" s="7">
+        <v>54</v>
+      </c>
+      <c r="D219" s="7">
+        <v>3.45</v>
+      </c>
+      <c r="E219" s="7">
+        <v>0</v>
+      </c>
+      <c r="F219" s="7">
+        <v>0.02</v>
+      </c>
       <c r="G219" s="2"/>
     </row>
     <row r="220" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B220" s="2"/>
+      <c r="C220" s="7">
+        <v>55</v>
+      </c>
+      <c r="D220" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="E220" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F220" s="7">
+        <v>0</v>
+      </c>
       <c r="G220" s="2"/>
     </row>
     <row r="221" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B221" s="2"/>
+      <c r="C221" s="7">
+        <v>56</v>
+      </c>
+      <c r="D221" s="7">
+        <v>3.95</v>
+      </c>
+      <c r="E221" s="7">
+        <v>0</v>
+      </c>
+      <c r="F221" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G221" s="2"/>
     </row>
     <row r="222" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B222" s="2"/>
+      <c r="C222" s="7">
+        <v>57</v>
+      </c>
+      <c r="D222" s="7">
+        <v>2.98</v>
+      </c>
+      <c r="E222" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F222" s="7">
+        <v>0</v>
+      </c>
       <c r="G222" s="2"/>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B223" s="2"/>
+      <c r="C223" s="7">
+        <v>58</v>
+      </c>
+      <c r="D223" s="7">
+        <v>2.98</v>
+      </c>
+      <c r="E223" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F223" s="7">
+        <v>0</v>
+      </c>
       <c r="G223" s="2"/>
     </row>
     <row r="224" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B224" s="2"/>
+      <c r="C224" s="7">
+        <v>59</v>
+      </c>
+      <c r="D224" s="7">
+        <v>3.57</v>
+      </c>
+      <c r="E224" s="7">
+        <v>0</v>
+      </c>
+      <c r="F224" s="7">
+        <v>0.02</v>
+      </c>
       <c r="G224" s="2"/>
     </row>
     <row r="225" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B225" s="2"/>
+      <c r="C225" s="7">
+        <v>60</v>
+      </c>
+      <c r="D225" s="7">
+        <v>2.98</v>
+      </c>
+      <c r="E225" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F225" s="7">
+        <v>0</v>
+      </c>
       <c r="G225" s="2"/>
     </row>
     <row r="226" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B226" s="2"/>
+      <c r="C226" s="7">
+        <v>61</v>
+      </c>
+      <c r="D226" s="7">
+        <v>3</v>
+      </c>
+      <c r="E226" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F226" s="7">
+        <v>0.01</v>
+      </c>
       <c r="G226" s="2"/>
     </row>
     <row r="227" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B227" s="2"/>
+      <c r="C227" s="7">
+        <v>62</v>
+      </c>
+      <c r="D227" s="7">
+        <v>2.98</v>
+      </c>
+      <c r="E227" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F227" s="7">
+        <v>0</v>
+      </c>
       <c r="G227" s="2"/>
     </row>
     <row r="228" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B228" s="2"/>
+      <c r="C228" s="7">
+        <v>63</v>
+      </c>
+      <c r="D228" s="7">
+        <v>2.98</v>
+      </c>
+      <c r="E228" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F228" s="7">
+        <v>0</v>
+      </c>
       <c r="G228" s="2"/>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B229" s="2"/>
+      <c r="C229" s="7">
+        <v>64</v>
+      </c>
+      <c r="D229" s="7">
+        <v>2.98</v>
+      </c>
+      <c r="E229" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F229" s="7">
+        <v>0</v>
+      </c>
       <c r="G229" s="2"/>
     </row>
     <row r="230" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>